<commit_message>
filled NaN vals in prob table with 0s
</commit_message>
<xml_diff>
--- a/utility/data/pepsin/pepsin.xlsx
+++ b/utility/data/pepsin/pepsin.xlsx
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -643,10 +643,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="J3" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="T3" t="n">
         <v>0</v>
@@ -759,7 +759,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -847,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -890,19 +890,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -932,13 +932,13 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -1048,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -1133,13 +1133,13 @@
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -1158,19 +1158,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D11" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -1185,19 +1185,19 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L11" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="O11" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -1206,13 +1206,13 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="S11" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="T11" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
@@ -1228,13 +1228,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1255,7 +1255,7 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -1264,13 +1264,13 @@
         <v>0</v>
       </c>
       <c r="O12" t="n">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="P12" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q12" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="P13" t="n">
         <v>0</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -1389,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="R14" t="n">
         <v>0</v>
@@ -1429,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="R15" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -1505,29 +1505,29 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
+        <v>44</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>22</v>
       </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>11</v>
-      </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1569,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F17" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1596,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O17" t="n">
         <v>0</v>
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1672,13 +1672,13 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
+        <v>48</v>
+      </c>
+      <c r="R18" t="n">
         <v>24</v>
       </c>
-      <c r="R18" t="n">
-        <v>12</v>
-      </c>
       <c r="S18" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -1694,7 +1694,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -1706,7 +1706,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -2083,7 +2083,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -2095,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -2104,28 +2104,28 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
         <v>2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>3</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -2284,7 +2284,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -2308,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -2351,19 +2351,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -2442,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
@@ -2622,17 +2622,17 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
         <v>2</v>
       </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
@@ -2667,10 +2667,10 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -2689,13 +2689,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" t="n">
         <v>0</v>
@@ -2893,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
@@ -2966,7 +2966,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -3021,7 +3021,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -3030,10 +3030,10 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -3091,7 +3091,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -3109,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -3155,7 +3155,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -3167,7 +3167,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
reran small portion of data, refactored import statements
</commit_message>
<xml_diff>
--- a/utility/data/pepsin/pepsin.xlsx
+++ b/utility/data/pepsin/pepsin.xlsx
@@ -555,10 +555,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="C2" t="n">
-        <v>167</v>
+        <v>37</v>
       </c>
       <c r="D2" t="n">
         <v>9</v>
@@ -567,52 +567,52 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I2" t="n">
+        <v>10</v>
+      </c>
+      <c r="J2" t="n">
+        <v>26</v>
+      </c>
+      <c r="K2" t="n">
+        <v>13</v>
+      </c>
+      <c r="L2" t="n">
+        <v>21</v>
+      </c>
+      <c r="M2" t="n">
+        <v>16</v>
+      </c>
+      <c r="N2" t="n">
+        <v>28</v>
+      </c>
+      <c r="O2" t="n">
+        <v>75</v>
+      </c>
+      <c r="P2" t="n">
         <v>20</v>
       </c>
-      <c r="J2" t="n">
-        <v>63</v>
-      </c>
-      <c r="K2" t="n">
-        <v>34</v>
-      </c>
-      <c r="L2" t="n">
-        <v>68</v>
-      </c>
-      <c r="M2" t="n">
-        <v>64</v>
-      </c>
-      <c r="N2" t="n">
-        <v>52</v>
-      </c>
-      <c r="O2" t="n">
-        <v>166</v>
-      </c>
-      <c r="P2" t="n">
-        <v>62</v>
-      </c>
       <c r="Q2" t="n">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="R2" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="T2" t="n">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="U2" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -622,61 +622,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="C3" t="n">
-        <v>150</v>
+        <v>61</v>
       </c>
       <c r="D3" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E3" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="F3" t="n">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="I3" t="n">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="J3" t="n">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="K3" t="n">
         <v>13</v>
       </c>
       <c r="L3" t="n">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="M3" t="n">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="N3" t="n">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="O3" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="P3" t="n">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="Q3" t="n">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="R3" t="n">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="S3" t="n">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="T3" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="U3" t="n">
         <v>2</v>
@@ -689,10 +689,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D4" t="n">
         <v>10</v>
@@ -701,52 +701,52 @@
         <v>16</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="I4" t="n">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="J4" t="n">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="K4" t="n">
         <v>9</v>
       </c>
       <c r="L4" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>9</v>
       </c>
       <c r="N4" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="O4" t="n">
         <v>16</v>
       </c>
       <c r="P4" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q4" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="R4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="S4" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="U4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -756,64 +756,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C5" t="n">
-        <v>106</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F5" t="n">
-        <v>145</v>
+        <v>63</v>
       </c>
       <c r="G5" t="n">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="H5" t="n">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="I5" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J5" t="n">
-        <v>194</v>
+        <v>83</v>
       </c>
       <c r="K5" t="n">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="L5" t="n">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="M5" t="n">
+        <v>25</v>
+      </c>
+      <c r="N5" t="n">
+        <v>22</v>
+      </c>
+      <c r="O5" t="n">
         <v>55</v>
       </c>
-      <c r="N5" t="n">
-        <v>75</v>
-      </c>
-      <c r="O5" t="n">
-        <v>137</v>
-      </c>
       <c r="P5" t="n">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="Q5" t="n">
-        <v>137</v>
+        <v>84</v>
       </c>
       <c r="R5" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="S5" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="T5" t="n">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="U5" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>127</v>
+        <v>21</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
@@ -835,52 +835,52 @@
         <v>5</v>
       </c>
       <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25</v>
+      </c>
+      <c r="I6" t="n">
+        <v>15</v>
+      </c>
+      <c r="J6" t="n">
+        <v>28</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" t="n">
+        <v>15</v>
+      </c>
+      <c r="M6" t="n">
         <v>31</v>
       </c>
-      <c r="G6" t="n">
-        <v>10</v>
-      </c>
-      <c r="H6" t="n">
-        <v>44</v>
-      </c>
-      <c r="I6" t="n">
-        <v>35</v>
-      </c>
-      <c r="J6" t="n">
-        <v>98</v>
-      </c>
-      <c r="K6" t="n">
-        <v>14</v>
-      </c>
-      <c r="L6" t="n">
-        <v>30</v>
-      </c>
-      <c r="M6" t="n">
-        <v>87</v>
-      </c>
       <c r="N6" t="n">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="O6" t="n">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="P6" t="n">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="Q6" t="n">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="R6" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" t="n">
+        <v>4</v>
+      </c>
+      <c r="T6" t="n">
         <v>6</v>
       </c>
-      <c r="S6" t="n">
-        <v>21</v>
-      </c>
-      <c r="T6" t="n">
-        <v>12</v>
-      </c>
       <c r="U6" t="n">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -890,64 +890,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>119</v>
+        <v>57</v>
       </c>
       <c r="C7" t="n">
-        <v>260</v>
+        <v>67</v>
       </c>
       <c r="D7" t="n">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="E7" t="n">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="F7" t="n">
+        <v>13</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16</v>
+      </c>
+      <c r="H7" t="n">
+        <v>18</v>
+      </c>
+      <c r="I7" t="n">
+        <v>30</v>
+      </c>
+      <c r="J7" t="n">
+        <v>70</v>
+      </c>
+      <c r="K7" t="n">
+        <v>12</v>
+      </c>
+      <c r="L7" t="n">
+        <v>42</v>
+      </c>
+      <c r="M7" t="n">
+        <v>78</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5</v>
+      </c>
+      <c r="O7" t="n">
         <v>73</v>
       </c>
-      <c r="G7" t="n">
-        <v>30</v>
-      </c>
-      <c r="H7" t="n">
-        <v>48</v>
-      </c>
-      <c r="I7" t="n">
-        <v>104</v>
-      </c>
-      <c r="J7" t="n">
-        <v>154</v>
-      </c>
-      <c r="K7" t="n">
-        <v>57</v>
-      </c>
-      <c r="L7" t="n">
-        <v>80</v>
-      </c>
-      <c r="M7" t="n">
-        <v>128</v>
-      </c>
-      <c r="N7" t="n">
-        <v>69</v>
-      </c>
-      <c r="O7" t="n">
-        <v>151</v>
-      </c>
       <c r="P7" t="n">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="Q7" t="n">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="R7" t="n">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="S7" t="n">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="T7" t="n">
-        <v>179</v>
+        <v>52</v>
       </c>
       <c r="U7" t="n">
-        <v>163</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8">
@@ -957,64 +957,64 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="C8" t="n">
-        <v>351</v>
+        <v>107</v>
       </c>
       <c r="D8" t="n">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="E8" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
-        <v>203</v>
+        <v>69</v>
       </c>
       <c r="G8" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H8" t="n">
-        <v>105</v>
+        <v>19</v>
       </c>
       <c r="I8" t="n">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="J8" t="n">
-        <v>294</v>
+        <v>108</v>
       </c>
       <c r="K8" t="n">
-        <v>95</v>
+        <v>38</v>
       </c>
       <c r="L8" t="n">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="M8" t="n">
-        <v>212</v>
+        <v>103</v>
       </c>
       <c r="N8" t="n">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="O8" t="n">
-        <v>249</v>
+        <v>87</v>
       </c>
       <c r="P8" t="n">
-        <v>233</v>
+        <v>74</v>
       </c>
       <c r="Q8" t="n">
-        <v>124</v>
+        <v>11</v>
       </c>
       <c r="R8" t="n">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="S8" t="n">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="T8" t="n">
-        <v>181</v>
+        <v>63</v>
       </c>
       <c r="U8" t="n">
-        <v>105</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -1024,10 +1024,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="G9" t="n">
         <v>2</v>
@@ -1048,40 +1048,40 @@
         <v>5</v>
       </c>
       <c r="J9" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="K9" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>19</v>
+      </c>
+      <c r="P9" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
         <v>10</v>
       </c>
-      <c r="O9" t="n">
-        <v>29</v>
-      </c>
-      <c r="P9" t="n">
-        <v>37</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>30</v>
-      </c>
-      <c r="R9" t="n">
-        <v>10</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>18</v>
-      </c>
       <c r="U9" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1091,64 +1091,64 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="C10" t="n">
-        <v>394</v>
+        <v>184</v>
       </c>
       <c r="D10" t="n">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="E10" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F10" t="n">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="G10" t="n">
         <v>11</v>
       </c>
       <c r="H10" t="n">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="I10" t="n">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="J10" t="n">
-        <v>198</v>
+        <v>80</v>
       </c>
       <c r="K10" t="n">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="L10" t="n">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="M10" t="n">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="N10" t="n">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="O10" t="n">
-        <v>149</v>
+        <v>64</v>
       </c>
       <c r="P10" t="n">
-        <v>158</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="n">
-        <v>143</v>
+        <v>63</v>
       </c>
       <c r="R10" t="n">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="S10" t="n">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="T10" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="U10" t="n">
-        <v>162</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
@@ -1158,64 +1158,64 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>211</v>
+        <v>81</v>
       </c>
       <c r="D11" t="n">
-        <v>110</v>
+        <v>13</v>
       </c>
       <c r="E11" t="n">
         <v>8</v>
       </c>
       <c r="F11" t="n">
-        <v>181</v>
+        <v>75</v>
       </c>
       <c r="G11" t="n">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="H11" t="n">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="I11" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="J11" t="n">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="K11" t="n">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="L11" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="N11" t="n">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="O11" t="n">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="P11" t="n">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="R11" t="n">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="S11" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="U11" t="n">
-        <v>94</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12">
@@ -1225,64 +1225,64 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="D12" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E12" t="n">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="G12" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H12" t="n">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="I12" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="J12" t="n">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="K12" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L12" t="n">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="M12" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="N12" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="O12" t="n">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="P12" t="n">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="Q12" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="S12" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="T12" t="n">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="U12" t="n">
-        <v>106</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13">
@@ -1292,64 +1292,64 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>130</v>
+        <v>56</v>
       </c>
       <c r="D13" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="E13" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="G13" t="n">
         <v>10</v>
       </c>
       <c r="H13" t="n">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="I13" t="n">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="J13" t="n">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="K13" t="n">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="L13" t="n">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="M13" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="N13" t="n">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="O13" t="n">
-        <v>169</v>
+        <v>58</v>
       </c>
       <c r="P13" t="n">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="Q13" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="R13" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
       </c>
       <c r="T13" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="U13" t="n">
-        <v>118</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
@@ -1359,64 +1359,64 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C14" t="n">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="D14" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F14" t="n">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="I14" t="n">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="J14" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K14" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="L14" t="n">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="M14" t="n">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="N14" t="n">
         <v>8</v>
       </c>
       <c r="O14" t="n">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="P14" t="n">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="Q14" t="n">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="R14" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="S14" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="T14" t="n">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="U14" t="n">
-        <v>91</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -1426,64 +1426,64 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="D15" t="n">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E15" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G15" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H15" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="J15" t="n">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="K15" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="M15" t="n">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N15" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="O15" t="n">
-        <v>143</v>
+        <v>30</v>
       </c>
       <c r="P15" t="n">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="Q15" t="n">
-        <v>126</v>
+        <v>58</v>
       </c>
       <c r="R15" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="T15" t="n">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="U15" t="n">
-        <v>104</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
@@ -1493,64 +1493,64 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="D16" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E16" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="G16" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="H16" t="n">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="I16" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="J16" t="n">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="K16" t="n">
         <v>11</v>
       </c>
       <c r="L16" t="n">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="M16" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="O16" t="n">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="P16" t="n">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="Q16" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="R16" t="n">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="S16" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="T16" t="n">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="U16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -1560,61 +1560,61 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>7</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" t="n">
+        <v>7</v>
+      </c>
+      <c r="J17" t="n">
+        <v>38</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" t="n">
+        <v>17</v>
+      </c>
+      <c r="M17" t="n">
+        <v>9</v>
+      </c>
+      <c r="N17" t="n">
+        <v>8</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
         <v>12</v>
       </c>
-      <c r="F17" t="n">
-        <v>44</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
-        <v>8</v>
-      </c>
-      <c r="I17" t="n">
-        <v>13</v>
-      </c>
-      <c r="J17" t="n">
-        <v>71</v>
-      </c>
-      <c r="K17" t="n">
-        <v>2</v>
-      </c>
-      <c r="L17" t="n">
-        <v>90</v>
-      </c>
-      <c r="M17" t="n">
-        <v>18</v>
-      </c>
-      <c r="N17" t="n">
-        <v>67</v>
-      </c>
-      <c r="O17" t="n">
-        <v>37</v>
-      </c>
-      <c r="P17" t="n">
-        <v>54</v>
-      </c>
       <c r="Q17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="R17" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="S17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="U17" t="n">
         <v>0</v>
@@ -1627,64 +1627,64 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C18" t="n">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="D18" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="G18" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H18" t="n">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="I18" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="J18" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="K18" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M18" t="n">
         <v>29</v>
       </c>
       <c r="N18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="O18" t="n">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="P18" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="Q18" t="n">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="R18" t="n">
+        <v>8</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
         <v>21</v>
       </c>
-      <c r="S18" t="n">
-        <v>16</v>
-      </c>
-      <c r="T18" t="n">
-        <v>28</v>
-      </c>
       <c r="U18" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -1694,64 +1694,64 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
+        <v>11</v>
+      </c>
+      <c r="F19" t="n">
         <v>14</v>
       </c>
-      <c r="F19" t="n">
-        <v>70</v>
-      </c>
       <c r="G19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I19" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J19" t="n">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="K19" t="n">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="L19" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="M19" t="n">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="N19" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O19" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="P19" t="n">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="Q19" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="R19" t="n">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="S19" t="n">
+        <v>2</v>
+      </c>
+      <c r="T19" t="n">
         <v>14</v>
       </c>
-      <c r="T19" t="n">
-        <v>28</v>
-      </c>
       <c r="U19" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
@@ -1761,64 +1761,64 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C20" t="n">
-        <v>158</v>
+        <v>53</v>
       </c>
       <c r="D20" t="n">
+        <v>16</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
+        <v>21</v>
+      </c>
+      <c r="G20" t="n">
+        <v>25</v>
+      </c>
+      <c r="H20" t="n">
+        <v>16</v>
+      </c>
+      <c r="I20" t="n">
+        <v>12</v>
+      </c>
+      <c r="J20" t="n">
+        <v>61</v>
+      </c>
+      <c r="K20" t="n">
+        <v>15</v>
+      </c>
+      <c r="L20" t="n">
+        <v>26</v>
+      </c>
+      <c r="M20" t="n">
+        <v>19</v>
+      </c>
+      <c r="N20" t="n">
+        <v>20</v>
+      </c>
+      <c r="O20" t="n">
+        <v>8</v>
+      </c>
+      <c r="P20" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q20" t="n">
         <v>37</v>
       </c>
-      <c r="E20" t="n">
-        <v>23</v>
-      </c>
-      <c r="F20" t="n">
-        <v>68</v>
-      </c>
-      <c r="G20" t="n">
-        <v>31</v>
-      </c>
-      <c r="H20" t="n">
-        <v>30</v>
-      </c>
-      <c r="I20" t="n">
-        <v>49</v>
-      </c>
-      <c r="J20" t="n">
-        <v>89</v>
-      </c>
-      <c r="K20" t="n">
-        <v>41</v>
-      </c>
-      <c r="L20" t="n">
-        <v>81</v>
-      </c>
-      <c r="M20" t="n">
-        <v>100</v>
-      </c>
-      <c r="N20" t="n">
-        <v>48</v>
-      </c>
-      <c r="O20" t="n">
-        <v>70</v>
-      </c>
-      <c r="P20" t="n">
-        <v>109</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>62</v>
-      </c>
       <c r="R20" t="n">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="S20" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="T20" t="n">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="U20" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1828,64 +1828,64 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>171</v>
+        <v>69</v>
       </c>
       <c r="C21" t="n">
-        <v>310</v>
+        <v>108</v>
       </c>
       <c r="D21" t="n">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" t="n">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="G21" t="n">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="H21" t="n">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="I21" t="n">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="J21" t="n">
-        <v>187</v>
+        <v>44</v>
       </c>
       <c r="K21" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="L21" t="n">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="M21" t="n">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="N21" t="n">
-        <v>174</v>
+        <v>68</v>
       </c>
       <c r="O21" t="n">
-        <v>136</v>
+        <v>63</v>
       </c>
       <c r="P21" t="n">
-        <v>169</v>
+        <v>70</v>
       </c>
       <c r="Q21" t="n">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="R21" t="n">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="S21" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="T21" t="n">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="U21" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2016,10 +2016,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C2" t="n">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2028,37 +2028,37 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="n">
+        <v>15</v>
+      </c>
+      <c r="K2" t="n">
         <v>8</v>
       </c>
-      <c r="J2" t="n">
-        <v>30</v>
-      </c>
-      <c r="K2" t="n">
-        <v>16</v>
-      </c>
       <c r="L2" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="N2" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O2" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="P2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q2" t="n">
         <v>1</v>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
         <v>0</v>
@@ -2083,61 +2083,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C3" t="n">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="D3" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="F3" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="I3" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="J3" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K3" t="n">
         <v>5</v>
       </c>
       <c r="L3" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O3" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="P3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Q3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3" t="n">
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
@@ -2150,10 +2150,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
@@ -2162,25 +2162,25 @@
         <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J4" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="K4" t="n">
         <v>4</v>
       </c>
       <c r="L4" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>5</v>
@@ -2195,16 +2195,16 @@
         <v>1</v>
       </c>
       <c r="Q4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -2217,64 +2217,64 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
       <c r="F5" t="n">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G5" t="n">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="H5" t="n">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J5" t="n">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="K5" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="L5" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="M5" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="N5" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="P5" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="Q5" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2284,10 +2284,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2296,40 +2296,40 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>2</v>
       </c>
-      <c r="H6" t="n">
-        <v>5</v>
-      </c>
       <c r="I6" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J6" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="N6" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O6" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="P6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6" t="n">
         <v>0</v>
@@ -2351,64 +2351,64 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C7" t="n">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="D7" t="n">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" t="n">
         <v>9</v>
       </c>
-      <c r="F7" t="n">
-        <v>18</v>
-      </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" t="n">
+        <v>22</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5</v>
+      </c>
+      <c r="L7" t="n">
         <v>13</v>
       </c>
-      <c r="H7" t="n">
+      <c r="M7" t="n">
+        <v>14</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>23</v>
+      </c>
+      <c r="P7" t="n">
         <v>3</v>
       </c>
-      <c r="I7" t="n">
-        <v>26</v>
-      </c>
-      <c r="J7" t="n">
-        <v>34</v>
-      </c>
-      <c r="K7" t="n">
-        <v>10</v>
-      </c>
-      <c r="L7" t="n">
-        <v>20</v>
-      </c>
-      <c r="M7" t="n">
-        <v>23</v>
-      </c>
-      <c r="N7" t="n">
-        <v>2</v>
-      </c>
-      <c r="O7" t="n">
-        <v>38</v>
-      </c>
-      <c r="P7" t="n">
-        <v>15</v>
-      </c>
       <c r="Q7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -2418,61 +2418,61 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C8" t="n">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="D8" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="G8" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="I8" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J8" t="n">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="K8" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="L8" t="n">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="M8" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="N8" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O8" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="P8" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="Q8" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="U8" t="n">
         <v>2</v>
@@ -2485,10 +2485,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2497,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -2509,28 +2509,28 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
         <v>2</v>
       </c>
-      <c r="L9" t="n">
-        <v>3</v>
-      </c>
-      <c r="M9" t="n">
-        <v>4</v>
-      </c>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
         <v>0</v>
@@ -2552,58 +2552,58 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C10" t="n">
-        <v>151</v>
+        <v>69</v>
       </c>
       <c r="D10" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="G10" t="n">
         <v>7</v>
       </c>
       <c r="H10" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K10" t="n">
+        <v>9</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>7</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1</v>
+      </c>
+      <c r="O10" t="n">
         <v>5</v>
       </c>
-      <c r="J10" t="n">
-        <v>28</v>
-      </c>
-      <c r="K10" t="n">
-        <v>14</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>18</v>
-      </c>
-      <c r="N10" t="n">
-        <v>6</v>
-      </c>
-      <c r="O10" t="n">
-        <v>23</v>
-      </c>
       <c r="P10" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q10" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -2619,31 +2619,31 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>33</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>12</v>
+      </c>
+      <c r="I11" t="n">
         <v>8</v>
       </c>
-      <c r="C11" t="n">
-        <v>73</v>
-      </c>
-      <c r="D11" t="n">
-        <v>18</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>25</v>
-      </c>
-      <c r="G11" t="n">
-        <v>7</v>
-      </c>
-      <c r="H11" t="n">
-        <v>32</v>
-      </c>
-      <c r="I11" t="n">
-        <v>16</v>
-      </c>
       <c r="J11" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -2655,25 +2655,25 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
         <v>0</v>
@@ -2686,37 +2686,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="D12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
         <v>1</v>
@@ -2728,19 +2728,19 @@
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
         <v>0</v>
       </c>
       <c r="T12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" t="n">
         <v>0</v>
@@ -2753,31 +2753,31 @@
         </is>
       </c>
       <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>27</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
         <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>56</v>
-      </c>
-      <c r="D13" t="n">
-        <v>23</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>16</v>
       </c>
       <c r="G13" t="n">
         <v>2</v>
       </c>
       <c r="H13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -2786,14 +2786,14 @@
         <v>0</v>
       </c>
       <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>6</v>
+      </c>
+      <c r="O13" t="n">
         <v>2</v>
       </c>
-      <c r="N13" t="n">
-        <v>12</v>
-      </c>
-      <c r="O13" t="n">
-        <v>5</v>
-      </c>
       <c r="P13" t="n">
         <v>0</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="U13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2820,10 +2820,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C14" t="n">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -2832,43 +2832,43 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="L14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M14" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
         <v>2</v>
       </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>5</v>
-      </c>
       <c r="R14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -2887,52 +2887,52 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>9</v>
       </c>
       <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
         <v>4</v>
       </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>9</v>
-      </c>
-      <c r="J15" t="n">
-        <v>13</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" t="n">
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
         <v>5</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>7</v>
-      </c>
-      <c r="P15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>13</v>
       </c>
       <c r="R15" t="n">
         <v>0</v>
@@ -2954,52 +2954,52 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C16" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D16" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G16" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K16" t="n">
         <v>2</v>
       </c>
       <c r="L16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
         <v>3</v>
       </c>
       <c r="P16" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R16" t="n">
         <v>0</v>
@@ -3021,19 +3021,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -3042,10 +3042,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
@@ -3060,10 +3060,10 @@
         <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -3088,10 +3088,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -3100,22 +3100,22 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G18" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
         <v>0</v>
@@ -3130,7 +3130,7 @@
         <v>1</v>
       </c>
       <c r="P18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -3155,10 +3155,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -3167,10 +3167,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
@@ -3188,28 +3188,28 @@
         <v>0</v>
       </c>
       <c r="M19" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" t="n">
         <v>1</v>
       </c>
       <c r="P19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19" t="n">
         <v>0</v>
@@ -3222,61 +3222,61 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C20" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
         <v>5</v>
       </c>
-      <c r="F20" t="n">
-        <v>9</v>
-      </c>
       <c r="G20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H20" t="n">
         <v>0</v>
       </c>
       <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
+        <v>5</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="n">
         <v>2</v>
       </c>
-      <c r="J20" t="n">
-        <v>6</v>
-      </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>7</v>
-      </c>
       <c r="N20" t="n">
+        <v>1</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="n">
         <v>5</v>
       </c>
-      <c r="O20" t="n">
-        <v>7</v>
-      </c>
-      <c r="P20" t="n">
-        <v>8</v>
-      </c>
       <c r="Q20" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
       </c>
       <c r="T20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U20" t="n">
         <v>0</v>
@@ -3289,53 +3289,53 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C21" t="n">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D21" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" t="n">
+        <v>4</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" t="n">
+        <v>1</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q21" t="n">
         <v>5</v>
       </c>
-      <c r="G21" t="n">
-        <v>5</v>
-      </c>
-      <c r="H21" t="n">
-        <v>7</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" t="n">
-        <v>5</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>1</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>2</v>
-      </c>
-      <c r="O21" t="n">
-        <v>1</v>
-      </c>
-      <c r="P21" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>9</v>
-      </c>
       <c r="R21" t="n">
         <v>0</v>
       </c>
@@ -3343,10 +3343,10 @@
         <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>